<commit_message>
updated metadata and scripts
</commit_message>
<xml_diff>
--- a/Morph2022/data/metadata.xlsx
+++ b/Morph2022/data/metadata.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hkenned6\Documents\Melichrus\Morphology (morphometrics, PATN, DELTA)\Morphometrics_2021_2022\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hkenned6\Documents\Melichrus\Morphology (morphometrics, PATN, DELTA)\Helen\Morph2022\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="4" r:id="rId1"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3913" uniqueCount="955">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3914" uniqueCount="956">
   <si>
     <t>Character number</t>
   </si>
@@ -2951,6 +2951,9 @@
   </si>
   <si>
     <t xml:space="preserve">Measure from the boundary of where the white petiole meets green lamina in the central axis of leaf, most discernible on adaxial surface. Measure along central axis or if very curved along margin. Include the attachment surface. On some leaves the end of the lamina is more obvious as there is a pinching in, but not on all. Be guided by green but consider the pinch. </t>
+  </si>
+  <si>
+    <t>VLOOKUP(W16,raw_data.csv!$F$1:$G$91,2,FALSE)</t>
   </si>
 </sst>
 </file>
@@ -3466,7 +3469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD185"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -22464,10 +22467,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG130"/>
+  <dimension ref="A1:AG134"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="E136" sqref="E136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -35230,6 +35233,11 @@
       </c>
       <c r="AF130" s="3" t="s">
         <v>891</v>
+      </c>
+    </row>
+    <row r="134" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="D134" s="3" t="s">
+        <v>955</v>
       </c>
     </row>
   </sheetData>

</xml_diff>